<commit_message>
Added tidsreg for Tom
</commit_message>
<xml_diff>
--- a/08-Project-Management/Tidsregistrering/Tidsregistrering (Tom).xlsx
+++ b/08-Project-Management/Tidsregistrering/Tidsregistrering (Tom).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Navn</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Implementert OC1, og observer metoder til UC-1</t>
+  </si>
+  <si>
+    <t>2015/03/02</t>
+  </si>
+  <si>
+    <t>Bugfix og endringer I frame kode</t>
   </si>
 </sst>
 </file>
@@ -186,10 +192,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -293,6 +299,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>